<commit_message>
Add a solution from Early
</commit_message>
<xml_diff>
--- a/CH-116 Remove rows and colums.xlsx
+++ b/CH-116 Remove rows and colums.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E84E0E-7F0B-43D5-ADB7-357FF1A0A3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372284D6-ADF3-436D-B80D-7198988C2F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="Alt1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt1'!$J$2:$K$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$J$2:$K$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$J$2:$K$7</definedName>
   </definedNames>
@@ -63,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="9">
   <si>
     <t>Result</t>
   </si>
@@ -626,6 +628,55 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>189700</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>67195</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{333B7638-DAA6-7643-B00B-68CFA2334DFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2910840" y="2110740"/>
+          <a:ext cx="7916380" cy="3724795"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1144,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6953B061-69A0-4DFD-B670-596098262143}">
   <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1432,9 +1483,9 @@
       <c r="N12" t="str">
         <v>E</v>
       </c>
-      <c r="P12" s="5" cm="1">
-        <f t="array" ref="P12:S15">_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(K12),_xlfn.VSTACK(1,_xlfn.ANCHORARRAY(C13)))</f>
-        <v>0</v>
+      <c r="P12" s="5" t="str" cm="1">
+        <f t="array" ref="P12:S15">_xlfn.LET(_xlpm.z, _xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(K12),_xlfn.VSTACK(1,_xlfn.ANCHORARRAY(C13))),IF(_xlpm.z=0,"",_xlpm.z))</f>
+        <v/>
       </c>
       <c r="Q12" s="11" t="str">
         <v>A</v>
@@ -1596,4 +1647,337 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7BB4234-6298-477A-95F2-99DE1B4A384D}">
+  <dimension ref="A1:P31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.125" style="2" customWidth="1"/>
+    <col min="2" max="8" width="6.375" customWidth="1"/>
+    <col min="9" max="9" width="65.25" customWidth="1"/>
+    <col min="10" max="13" width="6.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="32"/>
+      <c r="J1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="32"/>
+      <c r="P1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13">
+        <v>38</v>
+      </c>
+      <c r="D3" s="19">
+        <v>90</v>
+      </c>
+      <c r="E3" s="14">
+        <v>47</v>
+      </c>
+      <c r="F3" s="19">
+        <v>31</v>
+      </c>
+      <c r="G3" s="14">
+        <v>53</v>
+      </c>
+      <c r="H3" s="23">
+        <v>31</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="13">
+        <v>38</v>
+      </c>
+      <c r="L3" s="14">
+        <v>47</v>
+      </c>
+      <c r="M3" s="15">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="27">
+        <v>42</v>
+      </c>
+      <c r="D4" s="20">
+        <v>98</v>
+      </c>
+      <c r="E4" s="20">
+        <v>15</v>
+      </c>
+      <c r="F4" s="20">
+        <v>12</v>
+      </c>
+      <c r="G4" s="20">
+        <v>34</v>
+      </c>
+      <c r="H4" s="24">
+        <v>99</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="16">
+        <v>53</v>
+      </c>
+      <c r="L4" s="6">
+        <v>22</v>
+      </c>
+      <c r="M4" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="16">
+        <v>53</v>
+      </c>
+      <c r="D5" s="20">
+        <v>22</v>
+      </c>
+      <c r="E5" s="6">
+        <v>22</v>
+      </c>
+      <c r="F5" s="20">
+        <v>37</v>
+      </c>
+      <c r="G5" s="6">
+        <v>12</v>
+      </c>
+      <c r="H5" s="24">
+        <v>83</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="17">
+        <v>12</v>
+      </c>
+      <c r="L5" s="7">
+        <v>18</v>
+      </c>
+      <c r="M5" s="8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="27">
+        <v>57</v>
+      </c>
+      <c r="D6" s="20">
+        <v>18</v>
+      </c>
+      <c r="E6" s="20">
+        <v>67</v>
+      </c>
+      <c r="F6" s="20">
+        <v>81</v>
+      </c>
+      <c r="G6" s="20">
+        <v>100</v>
+      </c>
+      <c r="H6" s="24">
+        <v>100</v>
+      </c>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+    </row>
+    <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="16">
+        <v>12</v>
+      </c>
+      <c r="D7" s="20">
+        <v>90</v>
+      </c>
+      <c r="E7" s="6">
+        <v>18</v>
+      </c>
+      <c r="F7" s="20">
+        <v>57</v>
+      </c>
+      <c r="G7" s="6">
+        <v>27</v>
+      </c>
+      <c r="H7" s="24">
+        <v>92</v>
+      </c>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B8" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="29">
+        <v>31</v>
+      </c>
+      <c r="D8" s="21">
+        <v>86</v>
+      </c>
+      <c r="E8" s="21">
+        <v>100</v>
+      </c>
+      <c r="F8" s="21">
+        <v>21</v>
+      </c>
+      <c r="G8" s="21">
+        <v>18</v>
+      </c>
+      <c r="H8" s="25">
+        <v>27</v>
+      </c>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C12" t="str" cm="1">
+        <f t="array" ref="C12:F15">_xlfn.LET(_xlpm.data,B2:G8,
+ _xlpm.cols,_xlfn.HSTACK(1,_xlfn.SEQUENCE(,COLUMNS(_xlpm.data)/2,2,2)),
+ _xlpm.rws,_xlfn.VSTACK(1,_xlfn.SEQUENCE(ROWS(_xlpm.data)/2,,2,2)),
+ _xlpm.out,_xlfn.CHOOSECOLS(_xlfn.CHOOSEROWS(_xlpm.data,_xlpm.rws),_xlpm.cols),
+ IF(_xlpm.out="","",_xlpm.out))</f>
+        <v/>
+      </c>
+      <c r="D12" t="str">
+        <v>A</v>
+      </c>
+      <c r="E12" t="str">
+        <v>C</v>
+      </c>
+      <c r="F12" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C13" t="str">
+        <v>A</v>
+      </c>
+      <c r="D13">
+        <v>38</v>
+      </c>
+      <c r="E13">
+        <v>47</v>
+      </c>
+      <c r="F13">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C14" t="str">
+        <v>C</v>
+      </c>
+      <c r="D14">
+        <v>53</v>
+      </c>
+      <c r="E14">
+        <v>22</v>
+      </c>
+      <c r="F14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C15" t="str">
+        <v>E</v>
+      </c>
+      <c r="D15">
+        <v>12</v>
+      </c>
+      <c r="E15">
+        <v>18</v>
+      </c>
+      <c r="F15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I31" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="J1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
My single function done
</commit_message>
<xml_diff>
--- a/CH-116 Remove rows and colums.xlsx
+++ b/CH-116 Remove rows and colums.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372284D6-ADF3-436D-B80D-7198988C2F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92530255-FEC1-4F3A-B8DD-93E705F0497D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Alt1" sheetId="3" r:id="rId3"/>
+    <sheet name="MySingleFunction" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt1'!$J$2:$K$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$J$2:$K$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">MySingleFunction!$J$2:$K$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$J$2:$K$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -65,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="9">
   <si>
     <t>Result</t>
   </si>
@@ -1196,7 +1198,7 @@
   <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1653,7 +1655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7BB4234-6298-477A-95F2-99DE1B4A384D}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -1980,4 +1982,526 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA940AE-66A6-4694-8A65-F7B0030569C0}">
+  <dimension ref="A1:S31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.125" style="2" customWidth="1"/>
+    <col min="2" max="8" width="6.375" customWidth="1"/>
+    <col min="9" max="9" width="2.625" customWidth="1"/>
+    <col min="10" max="10" width="6.375" customWidth="1"/>
+    <col min="11" max="11" width="10.125" customWidth="1"/>
+    <col min="12" max="13" width="6.375" customWidth="1"/>
+    <col min="15" max="16" width="10.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="32"/>
+      <c r="J1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="32"/>
+      <c r="P1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13">
+        <v>38</v>
+      </c>
+      <c r="D3" s="19">
+        <v>90</v>
+      </c>
+      <c r="E3" s="14">
+        <v>47</v>
+      </c>
+      <c r="F3" s="19">
+        <v>31</v>
+      </c>
+      <c r="G3" s="14">
+        <v>53</v>
+      </c>
+      <c r="H3" s="23">
+        <v>31</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="13">
+        <v>38</v>
+      </c>
+      <c r="L3" s="14">
+        <v>47</v>
+      </c>
+      <c r="M3" s="15">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="27">
+        <v>42</v>
+      </c>
+      <c r="D4" s="20">
+        <v>98</v>
+      </c>
+      <c r="E4" s="20">
+        <v>15</v>
+      </c>
+      <c r="F4" s="20">
+        <v>12</v>
+      </c>
+      <c r="G4" s="20">
+        <v>34</v>
+      </c>
+      <c r="H4" s="24">
+        <v>99</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="16">
+        <v>53</v>
+      </c>
+      <c r="L4" s="6">
+        <v>22</v>
+      </c>
+      <c r="M4" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="16">
+        <v>53</v>
+      </c>
+      <c r="D5" s="20">
+        <v>22</v>
+      </c>
+      <c r="E5" s="6">
+        <v>22</v>
+      </c>
+      <c r="F5" s="20">
+        <v>37</v>
+      </c>
+      <c r="G5" s="6">
+        <v>12</v>
+      </c>
+      <c r="H5" s="24">
+        <v>83</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="17">
+        <v>12</v>
+      </c>
+      <c r="L5" s="7">
+        <v>18</v>
+      </c>
+      <c r="M5" s="8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="27">
+        <v>57</v>
+      </c>
+      <c r="D6" s="20">
+        <v>18</v>
+      </c>
+      <c r="E6" s="20">
+        <v>67</v>
+      </c>
+      <c r="F6" s="20">
+        <v>81</v>
+      </c>
+      <c r="G6" s="20">
+        <v>100</v>
+      </c>
+      <c r="H6" s="24">
+        <v>100</v>
+      </c>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+    </row>
+    <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="16">
+        <v>12</v>
+      </c>
+      <c r="D7" s="20">
+        <v>90</v>
+      </c>
+      <c r="E7" s="6">
+        <v>18</v>
+      </c>
+      <c r="F7" s="20">
+        <v>57</v>
+      </c>
+      <c r="G7" s="6">
+        <v>27</v>
+      </c>
+      <c r="H7" s="24">
+        <v>92</v>
+      </c>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B8" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="29">
+        <v>31</v>
+      </c>
+      <c r="D8" s="21">
+        <v>86</v>
+      </c>
+      <c r="E8" s="21">
+        <v>100</v>
+      </c>
+      <c r="F8" s="21">
+        <v>21</v>
+      </c>
+      <c r="G8" s="21">
+        <v>18</v>
+      </c>
+      <c r="H8" s="25">
+        <v>27</v>
+      </c>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C12" cm="1">
+        <f t="array" ref="C12:H12">MOD(COLUMN(C2:H2)-2,2)</f>
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="K12" cm="1">
+        <f t="array" ref="K12:N18">_xlfn._xlws.FILTER(B2:H8,_xlfn.HSTACK(1,_xlfn.ANCHORARRAY(C12)))</f>
+        <v>0</v>
+      </c>
+      <c r="L12" t="str">
+        <v>A</v>
+      </c>
+      <c r="M12" t="str">
+        <v>C</v>
+      </c>
+      <c r="N12" t="str">
+        <v>E</v>
+      </c>
+      <c r="P12" s="5" t="str" cm="1">
+        <f t="array" ref="P12:S15">_xlfn.LET(_xlpm.z, _xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(K12),_xlfn.VSTACK(1,_xlfn.ANCHORARRAY(C13))),IF(_xlpm.z=0,"",_xlpm.z))</f>
+        <v/>
+      </c>
+      <c r="Q12" s="11" t="str">
+        <v>A</v>
+      </c>
+      <c r="R12" s="11" t="str">
+        <v>C</v>
+      </c>
+      <c r="S12" s="12" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C13" cm="1">
+        <f t="array" ref="C13:C18">MOD(ROW(C3:C8)-2,2)</f>
+        <v>1</v>
+      </c>
+      <c r="K13" t="str">
+        <v>A</v>
+      </c>
+      <c r="L13">
+        <v>38</v>
+      </c>
+      <c r="M13">
+        <v>47</v>
+      </c>
+      <c r="N13">
+        <v>53</v>
+      </c>
+      <c r="P13" s="9" t="str">
+        <v>A</v>
+      </c>
+      <c r="Q13" s="13">
+        <v>38</v>
+      </c>
+      <c r="R13" s="14">
+        <v>47</v>
+      </c>
+      <c r="S13" s="15">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="K14" t="str">
+        <v>B</v>
+      </c>
+      <c r="L14">
+        <v>42</v>
+      </c>
+      <c r="M14">
+        <v>15</v>
+      </c>
+      <c r="N14">
+        <v>34</v>
+      </c>
+      <c r="P14" s="9" t="str">
+        <v>C</v>
+      </c>
+      <c r="Q14" s="16">
+        <v>53</v>
+      </c>
+      <c r="R14" s="6">
+        <v>22</v>
+      </c>
+      <c r="S14" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="K15" t="str">
+        <v>C</v>
+      </c>
+      <c r="L15">
+        <v>53</v>
+      </c>
+      <c r="M15">
+        <v>22</v>
+      </c>
+      <c r="N15">
+        <v>12</v>
+      </c>
+      <c r="P15" s="10" t="str">
+        <v>E</v>
+      </c>
+      <c r="Q15" s="17">
+        <v>12</v>
+      </c>
+      <c r="R15" s="7">
+        <v>18</v>
+      </c>
+      <c r="S15" s="8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="K16" t="str">
+        <v>D</v>
+      </c>
+      <c r="L16">
+        <v>57</v>
+      </c>
+      <c r="M16">
+        <v>67</v>
+      </c>
+      <c r="N16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="K17" t="str">
+        <v>E</v>
+      </c>
+      <c r="L17">
+        <v>12</v>
+      </c>
+      <c r="M17">
+        <v>18</v>
+      </c>
+      <c r="N17">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="K18" t="str">
+        <v>F</v>
+      </c>
+      <c r="L18">
+        <v>31</v>
+      </c>
+      <c r="M18">
+        <v>100</v>
+      </c>
+      <c r="N18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="K21" s="5" t="str" cm="1">
+        <f t="array" ref="K21:N24">_xlfn.LET(
+_xlpm.rs, MOD(ROW(C3:C8)-2,2),
+_xlpm.cs, MOD(COLUMN(C2:H2)-2,2),
+_xlpm.z,  _xlfn._xlws.FILTER(_xlfn._xlws.FILTER(B2:H8,_xlfn.HSTACK(1,_xlpm.cs)),_xlfn.VSTACK(1,_xlpm.rs)),
+IF(_xlpm.z=0,"",_xlpm.z)
+)</f>
+        <v/>
+      </c>
+      <c r="L21" s="11" t="str">
+        <v>A</v>
+      </c>
+      <c r="M21" s="11" t="str">
+        <v>C</v>
+      </c>
+      <c r="N21" s="12" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="22" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="K22" s="9" t="str">
+        <v>A</v>
+      </c>
+      <c r="L22" s="13">
+        <v>38</v>
+      </c>
+      <c r="M22" s="14">
+        <v>47</v>
+      </c>
+      <c r="N22" s="15">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="K23" s="9" t="str">
+        <v>C</v>
+      </c>
+      <c r="L23" s="16">
+        <v>53</v>
+      </c>
+      <c r="M23" s="6">
+        <v>22</v>
+      </c>
+      <c r="N23" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="K24" s="10" t="str">
+        <v>E</v>
+      </c>
+      <c r="L24" s="17">
+        <v>12</v>
+      </c>
+      <c r="M24" s="7">
+        <v>18</v>
+      </c>
+      <c r="N24" s="8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="I31" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="J1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>